<commit_message>
feat: refactor and add init and fill scripts
</commit_message>
<xml_diff>
--- a/output/matches-23-assigned.xlsx
+++ b/output/matches-23-assigned.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Assignation marqueurs" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -32,9 +32,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-    <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy\ hh:mm"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -441,31 +440,31 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>336619</v>
+        <v>337248</v>
       </c>
       <c r="B2" t="str">
-        <v>F</v>
+        <v>H</v>
       </c>
       <c r="C2" t="str">
-        <v>4L</v>
+        <v>M18</v>
       </c>
       <c r="D2" t="str">
-        <v>2023 | 4L</v>
+        <v>2023 | M18</v>
       </c>
       <c r="E2" t="str">
-        <v>jeu.</v>
+        <v>sam.</v>
       </c>
       <c r="F2" s="1">
-        <v>45190.854166666664</v>
+        <v>45192.416666666664</v>
       </c>
       <c r="G2" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H2" t="str">
-        <v>Lausanne II F4</v>
+        <v>Lausanne M18G</v>
       </c>
       <c r="I2" t="str">
-        <v>Aigle F4</v>
+        <v>Haute-Broye M18G</v>
       </c>
       <c r="J2" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
@@ -476,34 +475,34 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>336711</v>
+        <v>337249</v>
       </c>
       <c r="B3" t="str">
-        <v>F</v>
+        <v>H</v>
       </c>
       <c r="C3" t="str">
-        <v>3L</v>
+        <v>M18</v>
       </c>
       <c r="D3" t="str">
-        <v>2023 | 3L</v>
+        <v>2023 | M18</v>
       </c>
       <c r="E3" t="str">
         <v>sam.</v>
       </c>
       <c r="F3" s="1">
-        <v>45192.70832175926</v>
+        <v>45192.45833332176</v>
       </c>
       <c r="G3" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H3" t="str">
-        <v>Lausanne I F3</v>
+        <v>Lausanne M18G</v>
       </c>
       <c r="I3" t="str">
-        <v>Orbe I F3</v>
+        <v>Haute-Broye M18G</v>
       </c>
       <c r="J3" t="str">
-        <v>Salle omnisports de Grand-Vennes 1-3</v>
+        <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K3" t="str">
         <v>Lausanne III M4</v>
@@ -511,34 +510,34 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>336725</v>
+        <v>337222</v>
       </c>
       <c r="B4" t="str">
-        <v>F</v>
+        <v>H</v>
       </c>
       <c r="C4" t="str">
-        <v>3L</v>
+        <v>M18</v>
       </c>
       <c r="D4" t="str">
-        <v>2023 | 3L</v>
+        <v>2023 | M18</v>
       </c>
       <c r="E4" t="str">
-        <v>ven.</v>
+        <v>dim.</v>
       </c>
       <c r="F4" s="1">
-        <v>45212.854166666664</v>
+        <v>45200.416666666664</v>
       </c>
       <c r="G4" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H4" t="str">
-        <v>Lausanne I F3</v>
+        <v>Lausanne M18G</v>
       </c>
       <c r="I4" t="str">
-        <v>Yverdon I F3</v>
+        <v>Lutry-Lavaux M18G</v>
       </c>
       <c r="J4" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
+        <v>Centre Sportif Unil SOS II Dorigny 1</v>
       </c>
       <c r="K4" t="str">
         <v>Lausanne III M4</v>
@@ -546,34 +545,34 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>336735</v>
+        <v>326422</v>
       </c>
       <c r="B5" t="str">
-        <v>F</v>
+        <v>H</v>
       </c>
       <c r="C5" t="str">
-        <v>3L</v>
+        <v>1L</v>
       </c>
       <c r="D5" t="str">
-        <v>2023 | 3L</v>
+        <v>2023 | 1L</v>
       </c>
       <c r="E5" t="str">
         <v>ven.</v>
       </c>
       <c r="F5" s="1">
-        <v>45240.86457175926</v>
+        <v>45226.854166666664</v>
       </c>
       <c r="G5" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H5" t="str">
-        <v>Lausanne I F3</v>
+        <v>VBC Lausanne</v>
       </c>
       <c r="I5" t="str">
-        <v>BOPP F3</v>
+        <v>VBC La Côte</v>
       </c>
       <c r="J5" t="str">
-        <v>Salle omnisports de Grand-Vennes 3</v>
+        <v>Salle omnisports de Grand-Vennes 1-3</v>
       </c>
       <c r="K5" t="str">
         <v>Lausanne III M4</v>
@@ -581,31 +580,31 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>337058</v>
+        <v>336932</v>
       </c>
       <c r="B6" t="str">
         <v>F</v>
       </c>
       <c r="C6" t="str">
-        <v>M19</v>
+        <v>M23</v>
       </c>
       <c r="D6" t="str">
-        <v>2023 | M19</v>
+        <v>2023 | M23</v>
       </c>
       <c r="E6" t="str">
         <v>ven.</v>
       </c>
       <c r="F6" s="1">
-        <v>45254.791666666664</v>
+        <v>45233.80208332176</v>
       </c>
       <c r="G6" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H6" t="str">
-        <v>Lausanne M19F</v>
+        <v>Lausanne M23F</v>
       </c>
       <c r="I6" t="str">
-        <v>Littoral M19F</v>
+        <v>Yverdon M23F</v>
       </c>
       <c r="J6" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
@@ -616,34 +615,34 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>336943</v>
+        <v>337235</v>
       </c>
       <c r="B7" t="str">
-        <v>F</v>
+        <v>H</v>
       </c>
       <c r="C7" t="str">
-        <v>M23</v>
+        <v>M18</v>
       </c>
       <c r="D7" t="str">
-        <v>2023 | M23</v>
+        <v>2023 | M18</v>
       </c>
       <c r="E7" t="str">
-        <v>ven.</v>
+        <v>sam.</v>
       </c>
       <c r="F7" s="1">
-        <v>45261.80207175926</v>
+        <v>45248.416666666664</v>
       </c>
       <c r="G7" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H7" t="str">
-        <v>Lausanne M23F</v>
+        <v>Lausanne M18G</v>
       </c>
       <c r="I7" t="str">
-        <v>Ecublens M23F</v>
+        <v>Haute-Broye M18G</v>
       </c>
       <c r="J7" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
+        <v>Salle de Sport de Corsy</v>
       </c>
       <c r="K7" t="str">
         <v>Lausanne III M4</v>
@@ -651,34 +650,34 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>336953</v>
+        <v>337273</v>
       </c>
       <c r="B8" t="str">
         <v>F</v>
       </c>
       <c r="C8" t="str">
-        <v>M23</v>
+        <v>M17</v>
       </c>
       <c r="D8" t="str">
-        <v>2023 | M23</v>
+        <v>2023 | M17</v>
       </c>
       <c r="E8" t="str">
-        <v>ven.</v>
+        <v>sam.</v>
       </c>
       <c r="F8" s="1">
-        <v>45282.80207175926</v>
+        <v>45255.45833332176</v>
       </c>
       <c r="G8" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H8" t="str">
-        <v>Lausanne M23F</v>
+        <v>Lausanne M17F</v>
       </c>
       <c r="I8" t="str">
-        <v>Cheseaux II M23F</v>
+        <v>Cheseaux I M17F</v>
       </c>
       <c r="J8" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
+        <v>Salle de gym Bois-Murat A1</v>
       </c>
       <c r="K8" t="str">
         <v>Lausanne III M4</v>
@@ -686,34 +685,34 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>336503</v>
+        <v>336765</v>
       </c>
       <c r="B9" t="str">
-        <v>H</v>
+        <v>F</v>
       </c>
       <c r="C9" t="str">
-        <v>2L</v>
+        <v>3L</v>
       </c>
       <c r="D9" t="str">
-        <v>2023 | 2L</v>
+        <v>2023 | 3L</v>
       </c>
       <c r="E9" t="str">
         <v>jeu.</v>
       </c>
       <c r="F9" s="1">
-        <v>45309.854166666664</v>
+        <v>45302.854166666664</v>
       </c>
       <c r="G9" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H9" t="str">
-        <v>Lausanne II M2</v>
+        <v>Lausanne I F3</v>
       </c>
       <c r="I9" t="str">
-        <v>LUC III M2</v>
+        <v>La Côte II F3</v>
       </c>
       <c r="J9" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
+        <v>Salle omnisports de Grand-Vennes 2</v>
       </c>
       <c r="K9" t="str">
         <v>Lausanne III M4</v>
@@ -721,34 +720,34 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>337293</v>
+        <v>336503</v>
       </c>
       <c r="B10" t="str">
-        <v>F</v>
+        <v>H</v>
       </c>
       <c r="C10" t="str">
-        <v>M17</v>
+        <v>2L</v>
       </c>
       <c r="D10" t="str">
-        <v>2023 | M17</v>
+        <v>2023 | 2L</v>
       </c>
       <c r="E10" t="str">
-        <v>sam.</v>
+        <v>jeu.</v>
       </c>
       <c r="F10" s="1">
-        <v>45325.416666666664</v>
+        <v>45309.854166666664</v>
       </c>
       <c r="G10" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H10" t="str">
-        <v>Lausanne M17F</v>
+        <v>Lausanne II M2</v>
       </c>
       <c r="I10" t="str">
-        <v>Epalinges M17M</v>
+        <v>LUC III M2</v>
       </c>
       <c r="J10" t="str">
-        <v>Salle du Collège</v>
+        <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K10" t="str">
         <v>Lausanne III M4</v>
@@ -756,34 +755,34 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>326496</v>
+        <v>336775</v>
       </c>
       <c r="B11" t="str">
-        <v>H</v>
+        <v>F</v>
       </c>
       <c r="C11" t="str">
-        <v>1L</v>
+        <v>3L</v>
       </c>
       <c r="D11" t="str">
-        <v>2023 | 1L</v>
+        <v>2023 | 3L</v>
       </c>
       <c r="E11" t="str">
-        <v>ven.</v>
+        <v>jeu.</v>
       </c>
       <c r="F11" s="1">
-        <v>45331.83332175926</v>
+        <v>45316.854166666664</v>
       </c>
       <c r="G11" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H11" t="str">
-        <v>VBC Lausanne</v>
+        <v>Lausanne I F3</v>
       </c>
       <c r="I11" t="str">
-        <v>VBC Fully</v>
+        <v>Sainte-Croix II F3</v>
       </c>
       <c r="J11" t="str">
-        <v>Salle omnisports de Grand-Vennes 1-3</v>
+        <v>Salle omnisports de Grand-Vennes 2</v>
       </c>
       <c r="K11" t="str">
         <v>Lausanne III M4</v>
@@ -791,7 +790,7 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>326513</v>
+        <v>326501</v>
       </c>
       <c r="B12" t="str">
         <v>H</v>
@@ -803,10 +802,10 @@
         <v>2023 | 1L</v>
       </c>
       <c r="E12" t="str">
-        <v>sam.</v>
+        <v>dim.</v>
       </c>
       <c r="F12" s="1">
-        <v>45353.666666666664</v>
+        <v>45340.666666666664</v>
       </c>
       <c r="G12" t="str">
         <v>VBC Lausanne</v>
@@ -815,7 +814,7 @@
         <v>VBC Lausanne</v>
       </c>
       <c r="I12" t="str">
-        <v>VBC Le Locle</v>
+        <v>VBC Delémont</v>
       </c>
       <c r="J12" t="str">
         <v>Salle omnisports de Grand-Vennes 1-3</v>
@@ -826,66 +825,66 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>336796</v>
+        <v>337258</v>
       </c>
       <c r="B13" t="str">
-        <v>F</v>
+        <v>H</v>
       </c>
       <c r="C13" t="str">
-        <v>3L</v>
+        <v>M18</v>
       </c>
       <c r="D13" t="str">
-        <v>2023 | 3L</v>
+        <v>2023 | M18</v>
       </c>
       <c r="E13" t="str">
-        <v>ven.</v>
+        <v>sam.</v>
       </c>
       <c r="F13" s="1">
-        <v>45359.875</v>
+        <v>45374.5</v>
       </c>
       <c r="G13" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H13" t="str">
-        <v>Lausanne I F3</v>
+        <v>Lausanne M18G</v>
       </c>
       <c r="I13" t="str">
-        <v>Epalinges II F3</v>
+        <v>LUC M18G</v>
       </c>
       <c r="J13" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K13" t="str">
-        <v>Lausanne III M4</v>
+        <v>Lausanne II F4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>336273</v>
+        <v>337260</v>
       </c>
       <c r="B14" t="str">
         <v>H</v>
       </c>
       <c r="C14" t="str">
-        <v>4L</v>
+        <v>M18</v>
       </c>
       <c r="D14" t="str">
-        <v>2023 | 4L</v>
+        <v>2023 | M18</v>
       </c>
       <c r="E14" t="str">
-        <v>mar.</v>
+        <v>sam.</v>
       </c>
       <c r="F14" s="1">
-        <v>45188.854166666664</v>
+        <v>45374.58333332176</v>
       </c>
       <c r="G14" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H14" t="str">
-        <v>Lausanne III M4</v>
+        <v>Lausanne M18G</v>
       </c>
       <c r="I14" t="str">
-        <v>La Côte IV M4</v>
+        <v>Lutry-Lavaux M18G</v>
       </c>
       <c r="J14" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
@@ -896,34 +895,34 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>326401</v>
+        <v>336725</v>
       </c>
       <c r="B15" t="str">
-        <v>H</v>
+        <v>F</v>
       </c>
       <c r="C15" t="str">
-        <v>1L</v>
+        <v>3L</v>
       </c>
       <c r="D15" t="str">
-        <v>2023 | 1L</v>
+        <v>2023 | 3L</v>
       </c>
       <c r="E15" t="str">
         <v>ven.</v>
       </c>
       <c r="F15" s="1">
-        <v>45198.854166666664</v>
+        <v>45212.854166666664</v>
       </c>
       <c r="G15" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H15" t="str">
-        <v>VBC Lausanne</v>
+        <v>Lausanne I F3</v>
       </c>
       <c r="I15" t="str">
-        <v>Colombier Volley</v>
+        <v>Yverdon I F3</v>
       </c>
       <c r="J15" t="str">
-        <v>Salle omnisports de Grand-Vennes 1-3</v>
+        <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K15" t="str">
         <v>Lausanne II F4</v>
@@ -931,31 +930,31 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>326422</v>
+        <v>336471</v>
       </c>
       <c r="B16" t="str">
         <v>H</v>
       </c>
       <c r="C16" t="str">
-        <v>1L</v>
+        <v>2L</v>
       </c>
       <c r="D16" t="str">
-        <v>2023 | 1L</v>
+        <v>2023 | 2L</v>
       </c>
       <c r="E16" t="str">
-        <v>ven.</v>
+        <v>sam.</v>
       </c>
       <c r="F16" s="1">
-        <v>45226.854166666664</v>
+        <v>45234.64583332176</v>
       </c>
       <c r="G16" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H16" t="str">
-        <v>VBC Lausanne</v>
+        <v>Lausanne II M2</v>
       </c>
       <c r="I16" t="str">
-        <v>VBC La Côte</v>
+        <v>Lutry-Lavaux II M2</v>
       </c>
       <c r="J16" t="str">
         <v>Salle omnisports de Grand-Vennes 1-3</v>
@@ -1001,34 +1000,34 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>336481</v>
+        <v>326439</v>
       </c>
       <c r="B18" t="str">
         <v>H</v>
       </c>
       <c r="C18" t="str">
-        <v>2L</v>
+        <v>1L</v>
       </c>
       <c r="D18" t="str">
-        <v>2023 | 2L</v>
+        <v>2023 | 1L</v>
       </c>
       <c r="E18" t="str">
-        <v>ven.</v>
+        <v>sam.</v>
       </c>
       <c r="F18" s="1">
-        <v>45254.86457175926</v>
+        <v>45248.666666666664</v>
       </c>
       <c r="G18" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H18" t="str">
-        <v>Lausanne II M2</v>
+        <v>VBC Lausanne</v>
       </c>
       <c r="I18" t="str">
-        <v>Bussigny M2</v>
+        <v>VBC Cheseaux</v>
       </c>
       <c r="J18" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
+        <v>Salle omnisports de Grand-Vennes 1-3</v>
       </c>
       <c r="K18" t="str">
         <v>Lausanne II F4</v>
@@ -1036,34 +1035,34 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>326454</v>
+        <v>337065</v>
       </c>
       <c r="B19" t="str">
-        <v>H</v>
+        <v>F</v>
       </c>
       <c r="C19" t="str">
-        <v>1L</v>
+        <v>M19</v>
       </c>
       <c r="D19" t="str">
-        <v>2023 | 1L</v>
+        <v>2023 | M19</v>
       </c>
       <c r="E19" t="str">
         <v>ven.</v>
       </c>
       <c r="F19" s="1">
-        <v>45261.854166666664</v>
+        <v>45268.791666666664</v>
       </c>
       <c r="G19" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H19" t="str">
-        <v>VBC Lausanne</v>
+        <v>Lausanne M19F</v>
       </c>
       <c r="I19" t="str">
-        <v>VBC Servette Star-Onex</v>
+        <v>Ecublens II M19F</v>
       </c>
       <c r="J19" t="str">
-        <v>Salle omnisports de Grand-Vennes 1-3</v>
+        <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K19" t="str">
         <v>Lausanne II F4</v>
@@ -1071,34 +1070,34 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>336495</v>
+        <v>326470</v>
       </c>
       <c r="B20" t="str">
         <v>H</v>
       </c>
       <c r="C20" t="str">
-        <v>2L</v>
+        <v>1L</v>
       </c>
       <c r="D20" t="str">
-        <v>2023 | 2L</v>
+        <v>2023 | 1L</v>
       </c>
       <c r="E20" t="str">
         <v>ven.</v>
       </c>
       <c r="F20" s="1">
-        <v>45282.875</v>
+        <v>45303.86458332176</v>
       </c>
       <c r="G20" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H20" t="str">
-        <v>Lausanne II M2</v>
+        <v>VBC Lausanne</v>
       </c>
       <c r="I20" t="str">
-        <v>Sainte-Croix M2</v>
+        <v>Chênois Genève Volleyball</v>
       </c>
       <c r="J20" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
+        <v>Salle omnisports de Grand-Vennes 1-3</v>
       </c>
       <c r="K20" t="str">
         <v>Lausanne II F4</v>
@@ -1141,34 +1140,34 @@
     </row>
     <row r="22">
       <c r="A22">
-        <v>336965</v>
+        <v>337293</v>
       </c>
       <c r="B22" t="str">
         <v>F</v>
       </c>
       <c r="C22" t="str">
-        <v>M23</v>
+        <v>M17</v>
       </c>
       <c r="D22" t="str">
-        <v>2023 | M23</v>
+        <v>2023 | M17</v>
       </c>
       <c r="E22" t="str">
-        <v>ven.</v>
+        <v>sam.</v>
       </c>
       <c r="F22" s="1">
-        <v>45324.80207175926</v>
+        <v>45325.416666666664</v>
       </c>
       <c r="G22" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H22" t="str">
-        <v>Lausanne M23F</v>
+        <v>Lausanne M17F</v>
       </c>
       <c r="I22" t="str">
-        <v>Aigle M23F</v>
+        <v>Epalinges M17M</v>
       </c>
       <c r="J22" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
+        <v>Salle du Collège</v>
       </c>
       <c r="K22" t="str">
         <v>Lausanne II F4</v>
@@ -1176,34 +1175,34 @@
     </row>
     <row r="23">
       <c r="A23">
-        <v>326501</v>
+        <v>337097</v>
       </c>
       <c r="B23" t="str">
-        <v>H</v>
+        <v>F</v>
       </c>
       <c r="C23" t="str">
-        <v>1L</v>
+        <v>M19</v>
       </c>
       <c r="D23" t="str">
-        <v>2023 | 1L</v>
+        <v>2023 | M19</v>
       </c>
       <c r="E23" t="str">
-        <v>dim.</v>
+        <v>ven.</v>
       </c>
       <c r="F23" s="1">
-        <v>45340.666666666664</v>
+        <v>45345.791666666664</v>
       </c>
       <c r="G23" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H23" t="str">
-        <v>VBC Lausanne</v>
+        <v>Lausanne M19F</v>
       </c>
       <c r="I23" t="str">
-        <v>VBC Delémont</v>
+        <v>Cossonay II M19F</v>
       </c>
       <c r="J23" t="str">
-        <v>Salle omnisports de Grand-Vennes 1-3</v>
+        <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K23" t="str">
         <v>Lausanne II F4</v>
@@ -1211,86 +1210,86 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>337253</v>
+        <v>336273</v>
       </c>
       <c r="B24" t="str">
         <v>H</v>
       </c>
       <c r="C24" t="str">
-        <v>M18</v>
+        <v>4L</v>
       </c>
       <c r="D24" t="str">
-        <v>2023 | M18</v>
+        <v>2023 | 4L</v>
       </c>
       <c r="E24" t="str">
-        <v>dim.</v>
+        <v>mar.</v>
       </c>
       <c r="F24" s="1">
-        <v>45354.45832175926</v>
+        <v>45188.854166666664</v>
       </c>
       <c r="G24" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H24" t="str">
+        <v>Lausanne III M4</v>
+      </c>
+      <c r="I24" t="str">
+        <v>La Côte IV M4</v>
+      </c>
+      <c r="J24" t="str">
+        <v>Salle omnisports de Grand-Vennes 1</v>
+      </c>
+      <c r="K24" t="str">
         <v>Lausanne M18G</v>
-      </c>
-      <c r="I24" t="str">
-        <v>Haute-Broye M18G</v>
-      </c>
-      <c r="J24" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
-      </c>
-      <c r="K24" t="str">
-        <v>Lausanne II F4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>337248</v>
+        <v>336619</v>
       </c>
       <c r="B25" t="str">
-        <v>H</v>
+        <v>F</v>
       </c>
       <c r="C25" t="str">
-        <v>M18</v>
+        <v>4L</v>
       </c>
       <c r="D25" t="str">
-        <v>2023 | M18</v>
+        <v>2023 | 4L</v>
       </c>
       <c r="E25" t="str">
-        <v>sam.</v>
+        <v>jeu.</v>
       </c>
       <c r="F25" s="1">
-        <v>45192.416666666664</v>
+        <v>45190.854166666664</v>
       </c>
       <c r="G25" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H25" t="str">
+        <v>Lausanne II F4</v>
+      </c>
+      <c r="I25" t="str">
+        <v>Aigle F4</v>
+      </c>
+      <c r="J25" t="str">
+        <v>Salle omnisports de Grand-Vennes 1</v>
+      </c>
+      <c r="K25" t="str">
         <v>Lausanne M18G</v>
-      </c>
-      <c r="I25" t="str">
-        <v>Haute-Broye M18G</v>
-      </c>
-      <c r="J25" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
-      </c>
-      <c r="K25" t="str">
-        <v>Lausanne II M2</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>336623</v>
+        <v>336715</v>
       </c>
       <c r="B26" t="str">
         <v>F</v>
       </c>
       <c r="C26" t="str">
-        <v>4L</v>
+        <v>3L</v>
       </c>
       <c r="D26" t="str">
-        <v>2023 | 4L</v>
+        <v>2023 | 3L</v>
       </c>
       <c r="E26" t="str">
         <v>jeu.</v>
@@ -1302,304 +1301,304 @@
         <v>VBC Lausanne</v>
       </c>
       <c r="H26" t="str">
-        <v>Lausanne II F4</v>
+        <v>Lausanne I F3</v>
       </c>
       <c r="I26" t="str">
-        <v>Littoral F4</v>
+        <v>Montreux II F3</v>
       </c>
       <c r="J26" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
+        <v>Salle omnisports de Grand-Vennes 2</v>
       </c>
       <c r="K26" t="str">
-        <v>Lausanne II M2</v>
+        <v>Lausanne M18G</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>336925</v>
+        <v>337061</v>
       </c>
       <c r="B27" t="str">
         <v>F</v>
       </c>
       <c r="C27" t="str">
-        <v>M23</v>
+        <v>M19</v>
       </c>
       <c r="D27" t="str">
-        <v>2023 | M23</v>
+        <v>2023 | M19</v>
       </c>
       <c r="E27" t="str">
-        <v>ven.</v>
+        <v>mar.</v>
       </c>
       <c r="F27" s="1">
-        <v>45205.80207175926</v>
+        <v>45258.791666666664</v>
       </c>
       <c r="G27" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H27" t="str">
-        <v>Lausanne M23F</v>
+        <v>Lausanne M19F</v>
       </c>
       <c r="I27" t="str">
-        <v>La Tour M23F</v>
+        <v>La Côte M19F</v>
       </c>
       <c r="J27" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
+        <v>Salle omnisports de Grand-Vennes 2</v>
       </c>
       <c r="K27" t="str">
-        <v>Lausanne II M2</v>
+        <v>Lausanne M18G</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>337235</v>
+        <v>336785</v>
       </c>
       <c r="B28" t="str">
-        <v>H</v>
+        <v>F</v>
       </c>
       <c r="C28" t="str">
-        <v>M18</v>
+        <v>3L</v>
       </c>
       <c r="D28" t="str">
-        <v>2023 | M18</v>
+        <v>2023 | 3L</v>
       </c>
       <c r="E28" t="str">
-        <v>sam.</v>
+        <v>jeu.</v>
       </c>
       <c r="F28" s="1">
-        <v>45248.416666666664</v>
+        <v>45330.854166666664</v>
       </c>
       <c r="G28" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H28" t="str">
+        <v>Lausanne I F3</v>
+      </c>
+      <c r="I28" t="str">
+        <v>Cossonay II F3</v>
+      </c>
+      <c r="J28" t="str">
+        <v>Salle omnisports de Grand-Vennes 2</v>
+      </c>
+      <c r="K28" t="str">
         <v>Lausanne M18G</v>
-      </c>
-      <c r="I28" t="str">
-        <v>Haute-Broye M18G</v>
-      </c>
-      <c r="J28" t="str">
-        <v>Salle de Sport de Corsy</v>
-      </c>
-      <c r="K28" t="str">
-        <v>Lausanne II M2</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>337273</v>
+        <v>336711</v>
       </c>
       <c r="B29" t="str">
         <v>F</v>
       </c>
       <c r="C29" t="str">
-        <v>M17</v>
+        <v>3L</v>
       </c>
       <c r="D29" t="str">
-        <v>2023 | M17</v>
+        <v>2023 | 3L</v>
       </c>
       <c r="E29" t="str">
         <v>sam.</v>
       </c>
       <c r="F29" s="1">
-        <v>45255.45832175926</v>
+        <v>45192.70833332176</v>
       </c>
       <c r="G29" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H29" t="str">
-        <v>Lausanne M17F</v>
+        <v>Lausanne I F3</v>
       </c>
       <c r="I29" t="str">
-        <v>Cheseaux I M17F</v>
+        <v>Orbe I F3</v>
       </c>
       <c r="J29" t="str">
-        <v>Salle de gym Bois-Murat A1</v>
+        <v>Salle omnisports de Grand-Vennes 1-3</v>
       </c>
       <c r="K29" t="str">
-        <v>Lausanne II M2</v>
+        <v>Lausanne M23F</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>337065</v>
+        <v>326454</v>
       </c>
       <c r="B30" t="str">
-        <v>F</v>
+        <v>H</v>
       </c>
       <c r="C30" t="str">
-        <v>M19</v>
+        <v>1L</v>
       </c>
       <c r="D30" t="str">
-        <v>2023 | M19</v>
+        <v>2023 | 1L</v>
       </c>
       <c r="E30" t="str">
         <v>ven.</v>
       </c>
       <c r="F30" s="1">
-        <v>45268.791666666664</v>
+        <v>45261.854166666664</v>
       </c>
       <c r="G30" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H30" t="str">
-        <v>Lausanne M19F</v>
+        <v>VBC Lausanne</v>
       </c>
       <c r="I30" t="str">
-        <v>Ecublens II M19F</v>
+        <v>VBC Servette Star-Onex</v>
       </c>
       <c r="J30" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
+        <v>Salle omnisports de Grand-Vennes 1-3</v>
       </c>
       <c r="K30" t="str">
-        <v>Lausanne II M2</v>
+        <v>Lausanne M23F</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>336327</v>
+        <v>336495</v>
       </c>
       <c r="B31" t="str">
         <v>H</v>
       </c>
       <c r="C31" t="str">
-        <v>4L</v>
+        <v>2L</v>
       </c>
       <c r="D31" t="str">
-        <v>2023 | 4L</v>
+        <v>2023 | 2L</v>
       </c>
       <c r="E31" t="str">
-        <v>mar.</v>
+        <v>ven.</v>
       </c>
       <c r="F31" s="1">
-        <v>45300.854166666664</v>
+        <v>45282.875</v>
       </c>
       <c r="G31" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H31" t="str">
-        <v>Lausanne III M4</v>
+        <v>Lausanne II M2</v>
       </c>
       <c r="I31" t="str">
-        <v>Pailly M4</v>
+        <v>Sainte-Croix M2</v>
       </c>
       <c r="J31" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K31" t="str">
-        <v>Lausanne II M2</v>
+        <v>Lausanne M23F</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>326479</v>
+        <v>336511</v>
       </c>
       <c r="B32" t="str">
         <v>H</v>
       </c>
       <c r="C32" t="str">
-        <v>1L</v>
+        <v>2L</v>
       </c>
       <c r="D32" t="str">
-        <v>2023 | 1L</v>
+        <v>2023 | 2L</v>
       </c>
       <c r="E32" t="str">
-        <v>sam.</v>
+        <v>ven.</v>
       </c>
       <c r="F32" s="1">
-        <v>45311.666666666664</v>
+        <v>45324.875</v>
       </c>
       <c r="G32" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H32" t="str">
-        <v>VBC Lausanne</v>
+        <v>Lausanne II M2</v>
       </c>
       <c r="I32" t="str">
-        <v>TV Murten Volleyball</v>
+        <v>Littoral I M2</v>
       </c>
       <c r="J32" t="str">
-        <v>Salle omnisports de Grand-Vennes 1-3</v>
+        <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K32" t="str">
-        <v>Lausanne II M2</v>
+        <v>Lausanne M23F</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>336347</v>
+        <v>326496</v>
       </c>
       <c r="B33" t="str">
         <v>H</v>
       </c>
       <c r="C33" t="str">
-        <v>4L</v>
+        <v>1L</v>
       </c>
       <c r="D33" t="str">
-        <v>2023 | 4L</v>
+        <v>2023 | 1L</v>
       </c>
       <c r="E33" t="str">
-        <v>mar.</v>
+        <v>ven.</v>
       </c>
       <c r="F33" s="1">
-        <v>45328.854166666664</v>
+        <v>45331.83333332176</v>
       </c>
       <c r="G33" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H33" t="str">
-        <v>Lausanne III M4</v>
+        <v>VBC Lausanne</v>
       </c>
       <c r="I33" t="str">
-        <v>La Tour M4</v>
+        <v>VBC Fully</v>
       </c>
       <c r="J33" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
+        <v>Salle omnisports de Grand-Vennes 1-3</v>
       </c>
       <c r="K33" t="str">
-        <v>Lausanne II M2</v>
+        <v>Lausanne M23F</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>337301</v>
+        <v>336796</v>
       </c>
       <c r="B34" t="str">
         <v>F</v>
       </c>
       <c r="C34" t="str">
-        <v>M17</v>
+        <v>3L</v>
       </c>
       <c r="D34" t="str">
-        <v>2023 | M17</v>
+        <v>2023 | 3L</v>
       </c>
       <c r="E34" t="str">
-        <v>sam.</v>
+        <v>ven.</v>
       </c>
       <c r="F34" s="1">
-        <v>45346.375</v>
+        <v>45359.875</v>
       </c>
       <c r="G34" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H34" t="str">
-        <v>Lausanne M17F</v>
+        <v>Lausanne I F3</v>
       </c>
       <c r="I34" t="str">
-        <v>La Côte M17F</v>
+        <v>Epalinges II F3</v>
       </c>
       <c r="J34" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K34" t="str">
-        <v>Lausanne II M2</v>
+        <v>Lausanne M23F</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>336358</v>
+        <v>336623</v>
       </c>
       <c r="B35" t="str">
-        <v>H</v>
+        <v>F</v>
       </c>
       <c r="C35" t="str">
         <v>4L</v>
@@ -1608,383 +1607,383 @@
         <v>2023 | 4L</v>
       </c>
       <c r="E35" t="str">
-        <v>mar.</v>
+        <v>jeu.</v>
       </c>
       <c r="F35" s="1">
-        <v>45356.854166666664</v>
+        <v>45197.854166666664</v>
       </c>
       <c r="G35" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H35" t="str">
-        <v>Lausanne III M4</v>
+        <v>Lausanne II F4</v>
       </c>
       <c r="I35" t="str">
-        <v>La Côte III M4</v>
+        <v>Littoral F4</v>
       </c>
       <c r="J35" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K35" t="str">
-        <v>Lausanne II M2</v>
+        <v>Lausanne M23F</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>337249</v>
+        <v>336297</v>
       </c>
       <c r="B36" t="str">
         <v>H</v>
       </c>
       <c r="C36" t="str">
-        <v>M18</v>
+        <v>4L</v>
       </c>
       <c r="D36" t="str">
-        <v>2023 | M18</v>
+        <v>2023 | 4L</v>
       </c>
       <c r="E36" t="str">
-        <v>sam.</v>
+        <v>mar.</v>
       </c>
       <c r="F36" s="1">
-        <v>45192.45832175926</v>
+        <v>45237.854166666664</v>
       </c>
       <c r="G36" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H36" t="str">
-        <v>Lausanne M18G</v>
+        <v>Lausanne III M4</v>
       </c>
       <c r="I36" t="str">
-        <v>Haute-Broye M18G</v>
+        <v>Ecublens M4</v>
       </c>
       <c r="J36" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K36" t="str">
-        <v>Lausanne M19F</v>
+        <v>Lausanne M23F</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>337222</v>
+        <v>336309</v>
       </c>
       <c r="B37" t="str">
         <v>H</v>
       </c>
       <c r="C37" t="str">
-        <v>M18</v>
+        <v>4L</v>
       </c>
       <c r="D37" t="str">
-        <v>2023 | M18</v>
+        <v>2023 | 4L</v>
       </c>
       <c r="E37" t="str">
-        <v>dim.</v>
+        <v>mar.</v>
       </c>
       <c r="F37" s="1">
-        <v>45200.416666666664</v>
+        <v>45258.854166666664</v>
       </c>
       <c r="G37" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H37" t="str">
-        <v>Lausanne M18G</v>
+        <v>Lausanne III M4</v>
       </c>
       <c r="I37" t="str">
-        <v>Lutry-Lavaux M18G</v>
+        <v>Lutry-Lavaux III M4</v>
       </c>
       <c r="J37" t="str">
-        <v>Centre Sportif Unil SOS II Dorigny 1</v>
+        <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K37" t="str">
-        <v>Lausanne M19F</v>
+        <v>Lausanne M23F</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>336932</v>
+        <v>336655</v>
       </c>
       <c r="B38" t="str">
         <v>F</v>
       </c>
       <c r="C38" t="str">
-        <v>M23</v>
+        <v>4L</v>
       </c>
       <c r="D38" t="str">
-        <v>2023 | M23</v>
+        <v>2023 | 4L</v>
       </c>
       <c r="E38" t="str">
-        <v>ven.</v>
+        <v>jeu.</v>
       </c>
       <c r="F38" s="1">
-        <v>45233.80207175926</v>
+        <v>45260.854166666664</v>
       </c>
       <c r="G38" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H38" t="str">
+        <v>Lausanne II F4</v>
+      </c>
+      <c r="I38" t="str">
+        <v>Lutry-Lavaux II F4</v>
+      </c>
+      <c r="J38" t="str">
+        <v>Salle omnisports de Grand-Vennes 1</v>
+      </c>
+      <c r="K38" t="str">
         <v>Lausanne M23F</v>
-      </c>
-      <c r="I38" t="str">
-        <v>Yverdon M23F</v>
-      </c>
-      <c r="J38" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
-      </c>
-      <c r="K38" t="str">
-        <v>Lausanne M19F</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>326439</v>
+        <v>336693</v>
       </c>
       <c r="B39" t="str">
-        <v>H</v>
+        <v>F</v>
       </c>
       <c r="C39" t="str">
-        <v>1L</v>
+        <v>4L</v>
       </c>
       <c r="D39" t="str">
-        <v>2023 | 1L</v>
+        <v>2023 | 4L</v>
       </c>
       <c r="E39" t="str">
-        <v>sam.</v>
+        <v>jeu.</v>
       </c>
       <c r="F39" s="1">
-        <v>45248.666666666664</v>
+        <v>45330.854166666664</v>
       </c>
       <c r="G39" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H39" t="str">
-        <v>VBC Lausanne</v>
+        <v>Lausanne II F4</v>
       </c>
       <c r="I39" t="str">
-        <v>VBC Cheseaux</v>
+        <v>Le Mont II F4</v>
       </c>
       <c r="J39" t="str">
-        <v>Salle omnisports de Grand-Vennes 1-3</v>
+        <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K39" t="str">
-        <v>Lausanne M19F</v>
+        <v>Lausanne M23F</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>336747</v>
+        <v>336358</v>
       </c>
       <c r="B40" t="str">
-        <v>F</v>
+        <v>H</v>
       </c>
       <c r="C40" t="str">
-        <v>3L</v>
+        <v>4L</v>
       </c>
       <c r="D40" t="str">
-        <v>2023 | 3L</v>
+        <v>2023 | 4L</v>
       </c>
       <c r="E40" t="str">
-        <v>jeu.</v>
+        <v>mar.</v>
       </c>
       <c r="F40" s="1">
-        <v>45260.854166666664</v>
+        <v>45356.854166666664</v>
       </c>
       <c r="G40" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H40" t="str">
-        <v>Lausanne I F3</v>
+        <v>Lausanne III M4</v>
       </c>
       <c r="I40" t="str">
-        <v>Cheseaux IV F3</v>
+        <v>La Côte III M4</v>
       </c>
       <c r="J40" t="str">
-        <v>Salle omnisports de Grand-Vennes 2</v>
+        <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K40" t="str">
-        <v>Lausanne M19F</v>
+        <v>Lausanne M23F</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
-        <v>336487</v>
+        <v>336920</v>
       </c>
       <c r="B41" t="str">
-        <v>H</v>
+        <v>F</v>
       </c>
       <c r="C41" t="str">
-        <v>2L</v>
+        <v>M23</v>
       </c>
       <c r="D41" t="str">
-        <v>2023 | 2L</v>
+        <v>2023 | M23</v>
       </c>
       <c r="E41" t="str">
-        <v>jeu.</v>
+        <v>sam.</v>
       </c>
       <c r="F41" s="1">
-        <v>45267.854166666664</v>
+        <v>45192.625</v>
       </c>
       <c r="G41" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H41" t="str">
-        <v>Lausanne II M2</v>
+        <v>Lausanne M23F</v>
       </c>
       <c r="I41" t="str">
-        <v>La Côte II M2</v>
+        <v>Ecublens M23F</v>
       </c>
       <c r="J41" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
+        <v>Salle omnisports de Grand-Vennes 1-3</v>
       </c>
       <c r="K41" t="str">
-        <v>Lausanne M19F</v>
+        <v>Lausanne I F3</v>
       </c>
     </row>
     <row r="42">
       <c r="A42">
-        <v>336765</v>
+        <v>337049</v>
       </c>
       <c r="B42" t="str">
         <v>F</v>
       </c>
       <c r="C42" t="str">
-        <v>3L</v>
+        <v>M19</v>
       </c>
       <c r="D42" t="str">
-        <v>2023 | 3L</v>
+        <v>2023 | M19</v>
       </c>
       <c r="E42" t="str">
-        <v>jeu.</v>
+        <v>ven.</v>
       </c>
       <c r="F42" s="1">
-        <v>45302.854166666664</v>
+        <v>45240.791666666664</v>
       </c>
       <c r="G42" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H42" t="str">
+        <v>Lausanne M19F</v>
+      </c>
+      <c r="I42" t="str">
+        <v>Sainte-Croix M19F</v>
+      </c>
+      <c r="J42" t="str">
+        <v>Salle omnisports de Grand-Vennes 1</v>
+      </c>
+      <c r="K42" t="str">
         <v>Lausanne I F3</v>
-      </c>
-      <c r="I42" t="str">
-        <v>La Côte II F3</v>
-      </c>
-      <c r="J42" t="str">
-        <v>Salle omnisports de Grand-Vennes 2</v>
-      </c>
-      <c r="K42" t="str">
-        <v>Lausanne M19F</v>
       </c>
     </row>
     <row r="43">
       <c r="A43">
-        <v>336337</v>
+        <v>336976</v>
       </c>
       <c r="B43" t="str">
-        <v>H</v>
+        <v>F</v>
       </c>
       <c r="C43" t="str">
-        <v>4L</v>
+        <v>M23</v>
       </c>
       <c r="D43" t="str">
-        <v>2023 | 4L</v>
+        <v>2023 | M23</v>
       </c>
       <c r="E43" t="str">
-        <v>mar.</v>
+        <v>ven.</v>
       </c>
       <c r="F43" s="1">
-        <v>45314.854166666664</v>
+        <v>45359.80208332176</v>
       </c>
       <c r="G43" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H43" t="str">
-        <v>Lausanne III M4</v>
+        <v>Lausanne M23F</v>
       </c>
       <c r="I43" t="str">
-        <v>Sugnens-Cugy II M4</v>
+        <v>La Tour M23F</v>
       </c>
       <c r="J43" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K43" t="str">
-        <v>Lausanne M19F</v>
+        <v>Lausanne I F3</v>
       </c>
     </row>
     <row r="44">
       <c r="A44">
-        <v>336511</v>
+        <v>336277</v>
       </c>
       <c r="B44" t="str">
         <v>H</v>
       </c>
       <c r="C44" t="str">
-        <v>2L</v>
+        <v>4L</v>
       </c>
       <c r="D44" t="str">
-        <v>2023 | 2L</v>
+        <v>2023 | 4L</v>
       </c>
       <c r="E44" t="str">
-        <v>ven.</v>
+        <v>mar.</v>
       </c>
       <c r="F44" s="1">
-        <v>45324.875</v>
+        <v>45195.854166666664</v>
       </c>
       <c r="G44" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H44" t="str">
-        <v>Lausanne II M2</v>
+        <v>Lausanne III M4</v>
       </c>
       <c r="I44" t="str">
-        <v>Littoral I M2</v>
+        <v>Montreux II M4</v>
       </c>
       <c r="J44" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K44" t="str">
-        <v>Lausanne M19F</v>
+        <v>Lausanne I F3</v>
       </c>
     </row>
     <row r="45">
       <c r="A45">
-        <v>336520</v>
+        <v>337037</v>
       </c>
       <c r="B45" t="str">
-        <v>H</v>
+        <v>F</v>
       </c>
       <c r="C45" t="str">
-        <v>2L</v>
+        <v>M19</v>
       </c>
       <c r="D45" t="str">
-        <v>2023 | 2L</v>
+        <v>2023 | M19</v>
       </c>
       <c r="E45" t="str">
-        <v>jeu.</v>
+        <v>mar.</v>
       </c>
       <c r="F45" s="1">
-        <v>45351.854166666664</v>
+        <v>45202.791666666664</v>
       </c>
       <c r="G45" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H45" t="str">
-        <v>Lausanne II M2</v>
+        <v>Lausanne M19F</v>
       </c>
       <c r="I45" t="str">
-        <v>Les Cèdres M2</v>
+        <v>La Côte M19F</v>
       </c>
       <c r="J45" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K45" t="str">
-        <v>Lausanne M19F</v>
+        <v>Lausanne I F3</v>
       </c>
     </row>
     <row r="46">
       <c r="A46">
-        <v>336704</v>
+        <v>336287</v>
       </c>
       <c r="B46" t="str">
-        <v>F</v>
+        <v>H</v>
       </c>
       <c r="C46" t="str">
         <v>4L</v>
@@ -1993,33 +1992,33 @@
         <v>2023 | 4L</v>
       </c>
       <c r="E46" t="str">
-        <v>jeu.</v>
+        <v>mar.</v>
       </c>
       <c r="F46" s="1">
-        <v>45358.854166666664</v>
+        <v>45209.854166666664</v>
       </c>
       <c r="G46" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H46" t="str">
-        <v>Lausanne II F4</v>
+        <v>Lausanne III M4</v>
       </c>
       <c r="I46" t="str">
-        <v>La Tour I F4</v>
+        <v>Le Mont II M4</v>
       </c>
       <c r="J46" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K46" t="str">
-        <v>Lausanne M19F</v>
+        <v>Lausanne I F3</v>
       </c>
     </row>
     <row r="47">
       <c r="A47">
-        <v>336277</v>
+        <v>336633</v>
       </c>
       <c r="B47" t="str">
-        <v>H</v>
+        <v>F</v>
       </c>
       <c r="C47" t="str">
         <v>4L</v>
@@ -2028,655 +2027,655 @@
         <v>2023 | 4L</v>
       </c>
       <c r="E47" t="str">
-        <v>mar.</v>
+        <v>jeu.</v>
       </c>
       <c r="F47" s="1">
-        <v>45195.854166666664</v>
+        <v>45211.854166666664</v>
       </c>
       <c r="G47" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H47" t="str">
-        <v>Lausanne III M4</v>
+        <v>Lausanne II F4</v>
       </c>
       <c r="I47" t="str">
-        <v>Montreux II M4</v>
+        <v>Yverdon II F4</v>
       </c>
       <c r="J47" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K47" t="str">
-        <v>Lausanne M18G</v>
+        <v>Lausanne I F3</v>
       </c>
     </row>
     <row r="48">
       <c r="A48">
-        <v>337049</v>
+        <v>336643</v>
       </c>
       <c r="B48" t="str">
         <v>F</v>
       </c>
       <c r="C48" t="str">
-        <v>M19</v>
+        <v>4L</v>
       </c>
       <c r="D48" t="str">
-        <v>2023 | M19</v>
+        <v>2023 | 4L</v>
       </c>
       <c r="E48" t="str">
-        <v>ven.</v>
+        <v>jeu.</v>
       </c>
       <c r="F48" s="1">
-        <v>45240.791666666664</v>
+        <v>45239.854166666664</v>
       </c>
       <c r="G48" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H48" t="str">
-        <v>Lausanne M19F</v>
+        <v>Lausanne II F4</v>
       </c>
       <c r="I48" t="str">
-        <v>Sainte-Croix M19F</v>
+        <v>Haute-Broye I F4</v>
       </c>
       <c r="J48" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K48" t="str">
-        <v>Lausanne M18G</v>
+        <v>Lausanne I F3</v>
       </c>
     </row>
     <row r="49">
       <c r="A49">
-        <v>326458</v>
+        <v>336487</v>
       </c>
       <c r="B49" t="str">
         <v>H</v>
       </c>
       <c r="C49" t="str">
-        <v>1L</v>
+        <v>2L</v>
       </c>
       <c r="D49" t="str">
-        <v>2023 | 1L</v>
+        <v>2023 | 2L</v>
       </c>
       <c r="E49" t="str">
-        <v>sam.</v>
+        <v>jeu.</v>
       </c>
       <c r="F49" s="1">
-        <v>45269.75</v>
+        <v>45267.854166666664</v>
       </c>
       <c r="G49" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H49" t="str">
-        <v>VBC Lausanne</v>
+        <v>Lausanne II M2</v>
       </c>
       <c r="I49" t="str">
-        <v>VBC Porrentruy</v>
+        <v>La Côte II M2</v>
       </c>
       <c r="J49" t="str">
-        <v>Salle omnisports du Vieux-Moulin</v>
+        <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K49" t="str">
-        <v>Lausanne M18G</v>
+        <v>Lausanne I F3</v>
       </c>
     </row>
     <row r="50">
       <c r="A50">
-        <v>326483</v>
+        <v>337286</v>
       </c>
       <c r="B50" t="str">
-        <v>H</v>
+        <v>F</v>
       </c>
       <c r="C50" t="str">
-        <v>1L</v>
+        <v>M17</v>
       </c>
       <c r="D50" t="str">
-        <v>2023 | 1L</v>
+        <v>2023 | M17</v>
       </c>
       <c r="E50" t="str">
-        <v>ven.</v>
+        <v>mar.</v>
       </c>
       <c r="F50" s="1">
-        <v>45317.854166666664</v>
+        <v>45272.791666666664</v>
       </c>
       <c r="G50" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H50" t="str">
-        <v>VBC Lausanne</v>
+        <v>Lausanne M17F</v>
       </c>
       <c r="I50" t="str">
-        <v>Groupement Sportif du CERN</v>
+        <v>Lutry-Lavaux M17F</v>
       </c>
       <c r="J50" t="str">
-        <v>Salle omnisports de Grand-Vennes 1-3</v>
+        <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K50" t="str">
-        <v>Lausanne M18G</v>
+        <v>Lausanne I F3</v>
       </c>
     </row>
     <row r="51">
       <c r="A51">
-        <v>336976</v>
+        <v>337301</v>
       </c>
       <c r="B51" t="str">
         <v>F</v>
       </c>
       <c r="C51" t="str">
-        <v>M23</v>
+        <v>M17</v>
       </c>
       <c r="D51" t="str">
-        <v>2023 | M23</v>
+        <v>2023 | M17</v>
       </c>
       <c r="E51" t="str">
-        <v>ven.</v>
+        <v>sam.</v>
       </c>
       <c r="F51" s="1">
-        <v>45359.80207175926</v>
+        <v>45346.375</v>
       </c>
       <c r="G51" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H51" t="str">
-        <v>Lausanne M23F</v>
+        <v>Lausanne M17F</v>
       </c>
       <c r="I51" t="str">
-        <v>La Tour M23F</v>
+        <v>La Côte M17F</v>
       </c>
       <c r="J51" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K51" t="str">
-        <v>Lausanne M18G</v>
+        <v>Lausanne I F3</v>
       </c>
     </row>
     <row r="52">
       <c r="A52">
-        <v>336715</v>
+        <v>336704</v>
       </c>
       <c r="B52" t="str">
         <v>F</v>
       </c>
       <c r="C52" t="str">
-        <v>3L</v>
+        <v>4L</v>
       </c>
       <c r="D52" t="str">
-        <v>2023 | 3L</v>
+        <v>2023 | 4L</v>
       </c>
       <c r="E52" t="str">
         <v>jeu.</v>
       </c>
       <c r="F52" s="1">
-        <v>45197.854166666664</v>
+        <v>45358.854166666664</v>
       </c>
       <c r="G52" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H52" t="str">
+        <v>Lausanne II F4</v>
+      </c>
+      <c r="I52" t="str">
+        <v>La Tour I F4</v>
+      </c>
+      <c r="J52" t="str">
+        <v>Salle omnisports de Grand-Vennes 1</v>
+      </c>
+      <c r="K52" t="str">
         <v>Lausanne I F3</v>
-      </c>
-      <c r="I52" t="str">
-        <v>Montreux II F3</v>
-      </c>
-      <c r="J52" t="str">
-        <v>Salle omnisports de Grand-Vennes 2</v>
-      </c>
-      <c r="K52" t="str">
-        <v>Lausanne M23F</v>
       </c>
     </row>
     <row r="53">
       <c r="A53">
-        <v>337037</v>
+        <v>326401</v>
       </c>
       <c r="B53" t="str">
-        <v>F</v>
+        <v>H</v>
       </c>
       <c r="C53" t="str">
-        <v>M19</v>
+        <v>1L</v>
       </c>
       <c r="D53" t="str">
-        <v>2023 | M19</v>
+        <v>2023 | 1L</v>
       </c>
       <c r="E53" t="str">
-        <v>mar.</v>
+        <v>ven.</v>
       </c>
       <c r="F53" s="1">
-        <v>45202.791666666664</v>
+        <v>45198.854166666664</v>
       </c>
       <c r="G53" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H53" t="str">
+        <v>VBC Lausanne</v>
+      </c>
+      <c r="I53" t="str">
+        <v>Colombier Volley</v>
+      </c>
+      <c r="J53" t="str">
+        <v>Salle omnisports de Grand-Vennes 1-3</v>
+      </c>
+      <c r="K53" t="str">
         <v>Lausanne M19F</v>
-      </c>
-      <c r="I53" t="str">
-        <v>La Côte M19F</v>
-      </c>
-      <c r="J53" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
-      </c>
-      <c r="K53" t="str">
-        <v>Lausanne M23F</v>
       </c>
     </row>
     <row r="54">
       <c r="A54">
-        <v>336471</v>
+        <v>336735</v>
       </c>
       <c r="B54" t="str">
-        <v>H</v>
+        <v>F</v>
       </c>
       <c r="C54" t="str">
-        <v>2L</v>
+        <v>3L</v>
       </c>
       <c r="D54" t="str">
-        <v>2023 | 2L</v>
+        <v>2023 | 3L</v>
       </c>
       <c r="E54" t="str">
-        <v>sam.</v>
+        <v>ven.</v>
       </c>
       <c r="F54" s="1">
-        <v>45234.64582175926</v>
+        <v>45240.86458332176</v>
       </c>
       <c r="G54" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H54" t="str">
-        <v>Lausanne II M2</v>
+        <v>Lausanne I F3</v>
       </c>
       <c r="I54" t="str">
-        <v>Lutry-Lavaux II M2</v>
+        <v>BOPP F3</v>
       </c>
       <c r="J54" t="str">
-        <v>Salle omnisports de Grand-Vennes 1-3</v>
+        <v>Salle omnisports de Grand-Vennes 3</v>
       </c>
       <c r="K54" t="str">
-        <v>Lausanne M23F</v>
+        <v>Lausanne M19F</v>
       </c>
     </row>
     <row r="55">
       <c r="A55">
-        <v>337237</v>
+        <v>336481</v>
       </c>
       <c r="B55" t="str">
         <v>H</v>
       </c>
       <c r="C55" t="str">
-        <v>M18</v>
+        <v>2L</v>
       </c>
       <c r="D55" t="str">
-        <v>2023 | M18</v>
+        <v>2023 | 2L</v>
       </c>
       <c r="E55" t="str">
-        <v>dim.</v>
+        <v>ven.</v>
       </c>
       <c r="F55" s="1">
-        <v>45249.375</v>
+        <v>45254.86458332176</v>
       </c>
       <c r="G55" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H55" t="str">
-        <v>Lausanne M18G</v>
+        <v>Lausanne II M2</v>
       </c>
       <c r="I55" t="str">
-        <v>La Côte M18G</v>
+        <v>Bussigny M2</v>
       </c>
       <c r="J55" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K55" t="str">
-        <v>Lausanne M23F</v>
+        <v>Lausanne M19F</v>
       </c>
     </row>
     <row r="56">
       <c r="A56">
-        <v>337061</v>
+        <v>336491</v>
       </c>
       <c r="B56" t="str">
-        <v>F</v>
+        <v>H</v>
       </c>
       <c r="C56" t="str">
-        <v>M19</v>
+        <v>2L</v>
       </c>
       <c r="D56" t="str">
-        <v>2023 | M19</v>
+        <v>2023 | 2L</v>
       </c>
       <c r="E56" t="str">
-        <v>mar.</v>
+        <v>ven.</v>
       </c>
       <c r="F56" s="1">
-        <v>45258.791666666664</v>
+        <v>45275.86458332176</v>
       </c>
       <c r="G56" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H56" t="str">
+        <v>Lausanne II M2</v>
+      </c>
+      <c r="I56" t="str">
+        <v>Orbe M2</v>
+      </c>
+      <c r="J56" t="str">
+        <v>Salle omnisports de Grand-Vennes 1</v>
+      </c>
+      <c r="K56" t="str">
         <v>Lausanne M19F</v>
-      </c>
-      <c r="I56" t="str">
-        <v>La Côte M19F</v>
-      </c>
-      <c r="J56" t="str">
-        <v>Salle omnisports de Grand-Vennes 2</v>
-      </c>
-      <c r="K56" t="str">
-        <v>Lausanne M23F</v>
       </c>
     </row>
     <row r="57">
       <c r="A57">
-        <v>337286</v>
+        <v>326483</v>
       </c>
       <c r="B57" t="str">
-        <v>F</v>
+        <v>H</v>
       </c>
       <c r="C57" t="str">
-        <v>M17</v>
+        <v>1L</v>
       </c>
       <c r="D57" t="str">
-        <v>2023 | M17</v>
+        <v>2023 | 1L</v>
       </c>
       <c r="E57" t="str">
-        <v>mar.</v>
+        <v>ven.</v>
       </c>
       <c r="F57" s="1">
-        <v>45272.791666666664</v>
+        <v>45317.854166666664</v>
       </c>
       <c r="G57" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H57" t="str">
-        <v>Lausanne M17F</v>
+        <v>VBC Lausanne</v>
       </c>
       <c r="I57" t="str">
-        <v>Lutry-Lavaux M17F</v>
+        <v>Groupement Sportif du CERN</v>
       </c>
       <c r="J57" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
+        <v>Salle omnisports de Grand-Vennes 1-3</v>
       </c>
       <c r="K57" t="str">
-        <v>Lausanne M23F</v>
+        <v>Lausanne M19F</v>
       </c>
     </row>
     <row r="58">
       <c r="A58">
-        <v>336673</v>
+        <v>326513</v>
       </c>
       <c r="B58" t="str">
-        <v>F</v>
+        <v>H</v>
       </c>
       <c r="C58" t="str">
-        <v>4L</v>
+        <v>1L</v>
       </c>
       <c r="D58" t="str">
-        <v>2023 | 4L</v>
+        <v>2023 | 1L</v>
       </c>
       <c r="E58" t="str">
-        <v>jeu.</v>
+        <v>sam.</v>
       </c>
       <c r="F58" s="1">
-        <v>45302.854166666664</v>
+        <v>45353.666666666664</v>
       </c>
       <c r="G58" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H58" t="str">
-        <v>Lausanne II F4</v>
+        <v>VBC Lausanne</v>
       </c>
       <c r="I58" t="str">
-        <v>Pailly F4</v>
+        <v>VBC Le Locle</v>
       </c>
       <c r="J58" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
+        <v>Salle omnisports de Grand-Vennes 1-3</v>
       </c>
       <c r="K58" t="str">
-        <v>Lausanne M23F</v>
+        <v>Lausanne M19F</v>
       </c>
     </row>
     <row r="59">
       <c r="A59">
-        <v>336775</v>
+        <v>336925</v>
       </c>
       <c r="B59" t="str">
         <v>F</v>
       </c>
       <c r="C59" t="str">
-        <v>3L</v>
+        <v>M23</v>
       </c>
       <c r="D59" t="str">
-        <v>2023 | 3L</v>
+        <v>2023 | M23</v>
       </c>
       <c r="E59" t="str">
-        <v>jeu.</v>
+        <v>ven.</v>
       </c>
       <c r="F59" s="1">
-        <v>45316.854166666664</v>
+        <v>45205.80208332176</v>
       </c>
       <c r="G59" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H59" t="str">
-        <v>Lausanne I F3</v>
+        <v>Lausanne M23F</v>
       </c>
       <c r="I59" t="str">
-        <v>Sainte-Croix II F3</v>
+        <v>La Tour M23F</v>
       </c>
       <c r="J59" t="str">
-        <v>Salle omnisports de Grand-Vennes 2</v>
+        <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K59" t="str">
-        <v>Lausanne M23F</v>
+        <v>Lausanne M19F</v>
       </c>
     </row>
     <row r="60">
       <c r="A60">
-        <v>336785</v>
+        <v>336941</v>
       </c>
       <c r="B60" t="str">
         <v>F</v>
       </c>
       <c r="C60" t="str">
-        <v>3L</v>
+        <v>M23</v>
       </c>
       <c r="D60" t="str">
-        <v>2023 | 3L</v>
+        <v>2023 | M23</v>
       </c>
       <c r="E60" t="str">
         <v>jeu.</v>
       </c>
       <c r="F60" s="1">
-        <v>45330.854166666664</v>
+        <v>45253.80208332176</v>
       </c>
       <c r="G60" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H60" t="str">
-        <v>Lausanne I F3</v>
+        <v>Lausanne M23F</v>
       </c>
       <c r="I60" t="str">
-        <v>Cossonay II F3</v>
+        <v>Aigle M23F</v>
       </c>
       <c r="J60" t="str">
-        <v>Salle omnisports de Grand-Vennes 2</v>
+        <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K60" t="str">
-        <v>Lausanne M23F</v>
+        <v>Lausanne M19F</v>
       </c>
     </row>
     <row r="61">
       <c r="A61">
-        <v>337102</v>
+        <v>336747</v>
       </c>
       <c r="B61" t="str">
         <v>F</v>
       </c>
       <c r="C61" t="str">
-        <v>M19</v>
+        <v>3L</v>
       </c>
       <c r="D61" t="str">
-        <v>2023 | M19</v>
+        <v>2023 | 3L</v>
       </c>
       <c r="E61" t="str">
-        <v>sam.</v>
+        <v>jeu.</v>
       </c>
       <c r="F61" s="1">
-        <v>45353.5625</v>
+        <v>45260.854166666664</v>
       </c>
       <c r="G61" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H61" t="str">
+        <v>Lausanne I F3</v>
+      </c>
+      <c r="I61" t="str">
+        <v>Cheseaux IV F3</v>
+      </c>
+      <c r="J61" t="str">
+        <v>Salle omnisports de Grand-Vennes 2</v>
+      </c>
+      <c r="K61" t="str">
         <v>Lausanne M19F</v>
-      </c>
-      <c r="I61" t="str">
-        <v>Littoral M19F</v>
-      </c>
-      <c r="J61" t="str">
-        <v>Salle omnisports de Grand-Vennes 1-3</v>
-      </c>
-      <c r="K61" t="str">
-        <v>Lausanne M23F</v>
       </c>
     </row>
     <row r="62">
       <c r="A62">
-        <v>337258</v>
+        <v>336327</v>
       </c>
       <c r="B62" t="str">
         <v>H</v>
       </c>
       <c r="C62" t="str">
-        <v>M18</v>
+        <v>4L</v>
       </c>
       <c r="D62" t="str">
-        <v>2023 | M18</v>
+        <v>2023 | 4L</v>
       </c>
       <c r="E62" t="str">
-        <v>sam.</v>
+        <v>mar.</v>
       </c>
       <c r="F62" s="1">
-        <v>45374.5</v>
+        <v>45300.854166666664</v>
       </c>
       <c r="G62" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H62" t="str">
-        <v>Lausanne M18G</v>
+        <v>Lausanne III M4</v>
       </c>
       <c r="I62" t="str">
-        <v>LUC M18G</v>
+        <v>Pailly M4</v>
       </c>
       <c r="J62" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K62" t="str">
-        <v>Lausanne M23F</v>
+        <v>Lausanne M19F</v>
       </c>
     </row>
     <row r="63">
       <c r="A63">
-        <v>337033</v>
+        <v>336520</v>
       </c>
       <c r="B63" t="str">
-        <v>F</v>
+        <v>H</v>
       </c>
       <c r="C63" t="str">
-        <v>M19</v>
+        <v>2L</v>
       </c>
       <c r="D63" t="str">
-        <v>2023 | M19</v>
+        <v>2023 | 2L</v>
       </c>
       <c r="E63" t="str">
-        <v>ven.</v>
+        <v>jeu.</v>
       </c>
       <c r="F63" s="1">
-        <v>45198.78125</v>
+        <v>45351.854166666664</v>
       </c>
       <c r="G63" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H63" t="str">
+        <v>Lausanne II M2</v>
+      </c>
+      <c r="I63" t="str">
+        <v>Les Cèdres M2</v>
+      </c>
+      <c r="J63" t="str">
+        <v>Salle omnisports de Grand-Vennes 1</v>
+      </c>
+      <c r="K63" t="str">
         <v>Lausanne M19F</v>
-      </c>
-      <c r="I63" t="str">
-        <v>Yverdon M19F</v>
-      </c>
-      <c r="J63" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
-      </c>
-      <c r="K63" t="str">
-        <v>Lausanne I F3</v>
       </c>
     </row>
     <row r="64">
       <c r="A64">
-        <v>336287</v>
+        <v>337033</v>
       </c>
       <c r="B64" t="str">
-        <v>H</v>
+        <v>F</v>
       </c>
       <c r="C64" t="str">
-        <v>4L</v>
+        <v>M19</v>
       </c>
       <c r="D64" t="str">
-        <v>2023 | 4L</v>
+        <v>2023 | M19</v>
       </c>
       <c r="E64" t="str">
-        <v>mar.</v>
+        <v>ven.</v>
       </c>
       <c r="F64" s="1">
-        <v>45209.854166666664</v>
+        <v>45198.78125</v>
       </c>
       <c r="G64" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H64" t="str">
-        <v>Lausanne III M4</v>
+        <v>Lausanne M19F</v>
       </c>
       <c r="I64" t="str">
-        <v>Le Mont II M4</v>
+        <v>Yverdon M19F</v>
       </c>
       <c r="J64" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K64" t="str">
-        <v>Lausanne I F3</v>
+        <v>VBC Lausanne</v>
       </c>
     </row>
     <row r="65">
       <c r="A65">
-        <v>336297</v>
+        <v>337237</v>
       </c>
       <c r="B65" t="str">
         <v>H</v>
       </c>
       <c r="C65" t="str">
-        <v>4L</v>
+        <v>M18</v>
       </c>
       <c r="D65" t="str">
-        <v>2023 | 4L</v>
+        <v>2023 | M18</v>
       </c>
       <c r="E65" t="str">
-        <v>mar.</v>
+        <v>dim.</v>
       </c>
       <c r="F65" s="1">
-        <v>45237.854166666664</v>
+        <v>45249.375</v>
       </c>
       <c r="G65" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H65" t="str">
-        <v>Lausanne III M4</v>
+        <v>Lausanne M18G</v>
       </c>
       <c r="I65" t="str">
-        <v>Ecublens M4</v>
+        <v>La Côte M18G</v>
       </c>
       <c r="J65" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K65" t="str">
-        <v>Lausanne I F3</v>
+        <v>VBC Lausanne</v>
       </c>
     </row>
     <row r="66">
@@ -2711,47 +2710,47 @@
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K66" t="str">
-        <v>Lausanne I F3</v>
+        <v>VBC Lausanne</v>
       </c>
     </row>
     <row r="67">
       <c r="A67">
-        <v>336309</v>
+        <v>336943</v>
       </c>
       <c r="B67" t="str">
-        <v>H</v>
+        <v>F</v>
       </c>
       <c r="C67" t="str">
-        <v>4L</v>
+        <v>M23</v>
       </c>
       <c r="D67" t="str">
-        <v>2023 | 4L</v>
+        <v>2023 | M23</v>
       </c>
       <c r="E67" t="str">
-        <v>mar.</v>
+        <v>ven.</v>
       </c>
       <c r="F67" s="1">
-        <v>45258.854166666664</v>
+        <v>45261.80208332176</v>
       </c>
       <c r="G67" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H67" t="str">
-        <v>Lausanne III M4</v>
+        <v>Lausanne M23F</v>
       </c>
       <c r="I67" t="str">
-        <v>Lutry-Lavaux III M4</v>
+        <v>Ecublens M23F</v>
       </c>
       <c r="J67" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K67" t="str">
-        <v>Lausanne I F3</v>
+        <v>VBC Lausanne</v>
       </c>
     </row>
     <row r="68">
       <c r="A68">
-        <v>337069</v>
+        <v>337085</v>
       </c>
       <c r="B68" t="str">
         <v>F</v>
@@ -2766,7 +2765,7 @@
         <v>ven.</v>
       </c>
       <c r="F68" s="1">
-        <v>45275.791666666664</v>
+        <v>45317.78125</v>
       </c>
       <c r="G68" t="str">
         <v>VBC Lausanne</v>
@@ -2775,53 +2774,53 @@
         <v>Lausanne M19F</v>
       </c>
       <c r="I68" t="str">
-        <v>Ecublens II M19F</v>
+        <v>Orbe M19F</v>
       </c>
       <c r="J68" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K68" t="str">
-        <v>Lausanne I F3</v>
+        <v>VBC Lausanne</v>
       </c>
     </row>
     <row r="69">
       <c r="A69">
-        <v>326470</v>
+        <v>336967</v>
       </c>
       <c r="B69" t="str">
-        <v>H</v>
+        <v>F</v>
       </c>
       <c r="C69" t="str">
-        <v>1L</v>
+        <v>M23</v>
       </c>
       <c r="D69" t="str">
-        <v>2023 | 1L</v>
+        <v>2023 | M23</v>
       </c>
       <c r="E69" t="str">
         <v>ven.</v>
       </c>
       <c r="F69" s="1">
-        <v>45303.86457175926</v>
+        <v>45331.80208332176</v>
       </c>
       <c r="G69" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H69" t="str">
-        <v>VBC Lausanne</v>
+        <v>Lausanne M23F</v>
       </c>
       <c r="I69" t="str">
-        <v>Chênois Genève Volleyball</v>
+        <v>BOPP/Froidev II M23F</v>
       </c>
       <c r="J69" t="str">
-        <v>Salle omnisports de Grand-Vennes 1-3</v>
+        <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K69" t="str">
-        <v>Lausanne I F3</v>
+        <v>VBC Lausanne</v>
       </c>
     </row>
     <row r="70">
       <c r="A70">
-        <v>337085</v>
+        <v>337102</v>
       </c>
       <c r="B70" t="str">
         <v>F</v>
@@ -2833,10 +2832,10 @@
         <v>2023 | M19</v>
       </c>
       <c r="E70" t="str">
-        <v>ven.</v>
+        <v>sam.</v>
       </c>
       <c r="F70" s="1">
-        <v>45317.78125</v>
+        <v>45353.5625</v>
       </c>
       <c r="G70" t="str">
         <v>VBC Lausanne</v>
@@ -2845,228 +2844,228 @@
         <v>Lausanne M19F</v>
       </c>
       <c r="I70" t="str">
-        <v>Orbe M19F</v>
+        <v>Littoral M19F</v>
       </c>
       <c r="J70" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
+        <v>Salle omnisports de Grand-Vennes 1-3</v>
       </c>
       <c r="K70" t="str">
-        <v>Lausanne I F3</v>
+        <v>VBC Lausanne</v>
       </c>
     </row>
     <row r="71">
       <c r="A71">
-        <v>336967</v>
+        <v>336673</v>
       </c>
       <c r="B71" t="str">
         <v>F</v>
       </c>
       <c r="C71" t="str">
-        <v>M23</v>
+        <v>4L</v>
       </c>
       <c r="D71" t="str">
-        <v>2023 | M23</v>
+        <v>2023 | 4L</v>
       </c>
       <c r="E71" t="str">
-        <v>ven.</v>
+        <v>jeu.</v>
       </c>
       <c r="F71" s="1">
-        <v>45331.80207175926</v>
+        <v>45302.854166666664</v>
       </c>
       <c r="G71" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H71" t="str">
-        <v>Lausanne M23F</v>
+        <v>Lausanne II F4</v>
       </c>
       <c r="I71" t="str">
-        <v>BOPP/Froidev II M23F</v>
+        <v>Pailly F4</v>
       </c>
       <c r="J71" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K71" t="str">
-        <v>Lausanne I F3</v>
+        <v>VBC Lausanne</v>
       </c>
     </row>
     <row r="72">
       <c r="A72">
-        <v>337097</v>
+        <v>336337</v>
       </c>
       <c r="B72" t="str">
-        <v>F</v>
+        <v>H</v>
       </c>
       <c r="C72" t="str">
-        <v>M19</v>
+        <v>4L</v>
       </c>
       <c r="D72" t="str">
-        <v>2023 | M19</v>
+        <v>2023 | 4L</v>
       </c>
       <c r="E72" t="str">
-        <v>ven.</v>
+        <v>mar.</v>
       </c>
       <c r="F72" s="1">
-        <v>45345.791666666664</v>
+        <v>45314.854166666664</v>
       </c>
       <c r="G72" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H72" t="str">
-        <v>Lausanne M19F</v>
+        <v>Lausanne III M4</v>
       </c>
       <c r="I72" t="str">
-        <v>Cossonay II M19F</v>
+        <v>Sugnens-Cugy II M4</v>
       </c>
       <c r="J72" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K72" t="str">
-        <v>Lausanne I F3</v>
+        <v>VBC Lausanne</v>
       </c>
     </row>
     <row r="73">
       <c r="A73">
-        <v>337260</v>
+        <v>336683</v>
       </c>
       <c r="B73" t="str">
-        <v>H</v>
+        <v>F</v>
       </c>
       <c r="C73" t="str">
-        <v>M18</v>
+        <v>4L</v>
       </c>
       <c r="D73" t="str">
-        <v>2023 | M18</v>
+        <v>2023 | 4L</v>
       </c>
       <c r="E73" t="str">
-        <v>sam.</v>
+        <v>jeu.</v>
       </c>
       <c r="F73" s="1">
-        <v>45374.58332175926</v>
+        <v>45316.854166666664</v>
       </c>
       <c r="G73" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H73" t="str">
-        <v>Lausanne M18G</v>
+        <v>Lausanne II F4</v>
       </c>
       <c r="I73" t="str">
-        <v>Lutry-Lavaux M18G</v>
+        <v>Ecublens II F4</v>
       </c>
       <c r="J73" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K73" t="str">
-        <v>Lausanne I F3</v>
+        <v>VBC Lausanne</v>
       </c>
     </row>
     <row r="74">
       <c r="A74">
-        <v>336920</v>
+        <v>337058</v>
       </c>
       <c r="B74" t="str">
         <v>F</v>
       </c>
       <c r="C74" t="str">
-        <v>M23</v>
+        <v>M19</v>
       </c>
       <c r="D74" t="str">
-        <v>2023 | M23</v>
+        <v>2023 | M19</v>
       </c>
       <c r="E74" t="str">
-        <v>sam.</v>
+        <v>ven.</v>
       </c>
       <c r="F74" s="1">
-        <v>45192.625</v>
+        <v>45254.791666666664</v>
       </c>
       <c r="G74" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H74" t="str">
-        <v>Lausanne M23F</v>
+        <v>Lausanne M19F</v>
       </c>
       <c r="I74" t="str">
-        <v>Ecublens M23F</v>
+        <v>Littoral M19F</v>
       </c>
       <c r="J74" t="str">
-        <v>Salle omnisports de Grand-Vennes 1-3</v>
+        <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K74" t="str">
-        <v>VBC Lausanne</v>
+        <v>Lausanne II M2</v>
       </c>
     </row>
     <row r="75">
       <c r="A75">
-        <v>336633</v>
+        <v>337069</v>
       </c>
       <c r="B75" t="str">
         <v>F</v>
       </c>
       <c r="C75" t="str">
-        <v>4L</v>
+        <v>M19</v>
       </c>
       <c r="D75" t="str">
-        <v>2023 | 4L</v>
+        <v>2023 | M19</v>
       </c>
       <c r="E75" t="str">
-        <v>jeu.</v>
+        <v>ven.</v>
       </c>
       <c r="F75" s="1">
-        <v>45211.854166666664</v>
+        <v>45275.791666666664</v>
       </c>
       <c r="G75" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H75" t="str">
-        <v>Lausanne II F4</v>
+        <v>Lausanne M19F</v>
       </c>
       <c r="I75" t="str">
-        <v>Yverdon II F4</v>
+        <v>Ecublens II M19F</v>
       </c>
       <c r="J75" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K75" t="str">
-        <v>VBC Lausanne</v>
+        <v>Lausanne II M2</v>
       </c>
     </row>
     <row r="76">
       <c r="A76">
-        <v>336643</v>
+        <v>336953</v>
       </c>
       <c r="B76" t="str">
         <v>F</v>
       </c>
       <c r="C76" t="str">
-        <v>4L</v>
+        <v>M23</v>
       </c>
       <c r="D76" t="str">
-        <v>2023 | 4L</v>
+        <v>2023 | M23</v>
       </c>
       <c r="E76" t="str">
-        <v>jeu.</v>
+        <v>ven.</v>
       </c>
       <c r="F76" s="1">
-        <v>45239.854166666664</v>
+        <v>45282.80208332176</v>
       </c>
       <c r="G76" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H76" t="str">
-        <v>Lausanne II F4</v>
+        <v>Lausanne M23F</v>
       </c>
       <c r="I76" t="str">
-        <v>Haute-Broye I F4</v>
+        <v>Cheseaux II M23F</v>
       </c>
       <c r="J76" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K76" t="str">
-        <v>VBC Lausanne</v>
+        <v>Lausanne II M2</v>
       </c>
     </row>
     <row r="77">
       <c r="A77">
-        <v>336941</v>
+        <v>336965</v>
       </c>
       <c r="B77" t="str">
         <v>F</v>
@@ -3078,10 +3077,10 @@
         <v>2023 | M23</v>
       </c>
       <c r="E77" t="str">
-        <v>jeu.</v>
+        <v>ven.</v>
       </c>
       <c r="F77" s="1">
-        <v>45253.80207175926</v>
+        <v>45324.80208332176</v>
       </c>
       <c r="G77" t="str">
         <v>VBC Lausanne</v>
@@ -3096,217 +3095,217 @@
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K77" t="str">
-        <v>VBC Lausanne</v>
+        <v>Lausanne II M2</v>
       </c>
     </row>
     <row r="78">
       <c r="A78">
-        <v>336655</v>
+        <v>337255</v>
       </c>
       <c r="B78" t="str">
-        <v>F</v>
+        <v>H</v>
       </c>
       <c r="C78" t="str">
-        <v>4L</v>
+        <v>M18</v>
       </c>
       <c r="D78" t="str">
-        <v>2023 | 4L</v>
+        <v>2023 | M18</v>
       </c>
       <c r="E78" t="str">
-        <v>jeu.</v>
+        <v>dim.</v>
       </c>
       <c r="F78" s="1">
-        <v>45260.854166666664</v>
+        <v>45354.375</v>
       </c>
       <c r="G78" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H78" t="str">
-        <v>Lausanne II F4</v>
+        <v>Lausanne M18G</v>
       </c>
       <c r="I78" t="str">
-        <v>Lutry-Lavaux II F4</v>
+        <v>Lutry-Lavaux M18G</v>
       </c>
       <c r="J78" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K78" t="str">
-        <v>VBC Lausanne</v>
+        <v>Lausanne II M2</v>
       </c>
     </row>
     <row r="79">
       <c r="A79">
-        <v>336491</v>
+        <v>337253</v>
       </c>
       <c r="B79" t="str">
         <v>H</v>
       </c>
       <c r="C79" t="str">
-        <v>2L</v>
+        <v>M18</v>
       </c>
       <c r="D79" t="str">
-        <v>2023 | 2L</v>
+        <v>2023 | M18</v>
       </c>
       <c r="E79" t="str">
-        <v>ven.</v>
+        <v>dim.</v>
       </c>
       <c r="F79" s="1">
-        <v>45275.86457175926</v>
+        <v>45354.45833332176</v>
       </c>
       <c r="G79" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H79" t="str">
+        <v>Lausanne M18G</v>
+      </c>
+      <c r="I79" t="str">
+        <v>Haute-Broye M18G</v>
+      </c>
+      <c r="J79" t="str">
+        <v>Salle omnisports de Grand-Vennes 1</v>
+      </c>
+      <c r="K79" t="str">
         <v>Lausanne II M2</v>
-      </c>
-      <c r="I79" t="str">
-        <v>Orbe M2</v>
-      </c>
-      <c r="J79" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
-      </c>
-      <c r="K79" t="str">
-        <v>VBC Lausanne</v>
       </c>
     </row>
     <row r="80">
       <c r="A80">
-        <v>337288</v>
+        <v>326458</v>
       </c>
       <c r="B80" t="str">
-        <v>F</v>
+        <v>H</v>
       </c>
       <c r="C80" t="str">
-        <v>M17</v>
+        <v>1L</v>
       </c>
       <c r="D80" t="str">
-        <v>2023 | M17</v>
+        <v>2023 | 1L</v>
       </c>
       <c r="E80" t="str">
         <v>sam.</v>
       </c>
       <c r="F80" s="1">
-        <v>45304.45832175926</v>
+        <v>45269.75</v>
       </c>
       <c r="G80" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H80" t="str">
-        <v>Lausanne M17F</v>
+        <v>VBC Lausanne</v>
       </c>
       <c r="I80" t="str">
-        <v>Bussigny I M17F</v>
+        <v>VBC Porrentruy</v>
       </c>
       <c r="J80" t="str">
-        <v>Centre sportif Champs-de-la-Joux 2</v>
+        <v>Salle omnisports du Vieux-Moulin</v>
       </c>
       <c r="K80" t="str">
-        <v>VBC Lausanne</v>
+        <v>Lausanne II M2</v>
       </c>
     </row>
     <row r="81">
       <c r="A81">
-        <v>336683</v>
+        <v>337288</v>
       </c>
       <c r="B81" t="str">
         <v>F</v>
       </c>
       <c r="C81" t="str">
-        <v>4L</v>
+        <v>M17</v>
       </c>
       <c r="D81" t="str">
-        <v>2023 | 4L</v>
+        <v>2023 | M17</v>
       </c>
       <c r="E81" t="str">
-        <v>jeu.</v>
+        <v>sam.</v>
       </c>
       <c r="F81" s="1">
-        <v>45316.854166666664</v>
+        <v>45304.45833332176</v>
       </c>
       <c r="G81" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H81" t="str">
-        <v>Lausanne II F4</v>
+        <v>Lausanne M17F</v>
       </c>
       <c r="I81" t="str">
-        <v>Ecublens II F4</v>
+        <v>Bussigny I M17F</v>
       </c>
       <c r="J81" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
+        <v>Centre sportif Champs-de-la-Joux 2</v>
       </c>
       <c r="K81" t="str">
-        <v>VBC Lausanne</v>
+        <v>Lausanne II M2</v>
       </c>
     </row>
     <row r="82">
       <c r="A82">
-        <v>336693</v>
+        <v>326479</v>
       </c>
       <c r="B82" t="str">
-        <v>F</v>
+        <v>H</v>
       </c>
       <c r="C82" t="str">
-        <v>4L</v>
+        <v>1L</v>
       </c>
       <c r="D82" t="str">
-        <v>2023 | 4L</v>
+        <v>2023 | 1L</v>
       </c>
       <c r="E82" t="str">
-        <v>jeu.</v>
+        <v>sam.</v>
       </c>
       <c r="F82" s="1">
-        <v>45330.854166666664</v>
+        <v>45311.666666666664</v>
       </c>
       <c r="G82" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H82" t="str">
-        <v>Lausanne II F4</v>
+        <v>VBC Lausanne</v>
       </c>
       <c r="I82" t="str">
-        <v>Le Mont II F4</v>
+        <v>TV Murten Volleyball</v>
       </c>
       <c r="J82" t="str">
-        <v>Salle omnisports de Grand-Vennes 1</v>
+        <v>Salle omnisports de Grand-Vennes 1-3</v>
       </c>
       <c r="K82" t="str">
-        <v>VBC Lausanne</v>
+        <v>Lausanne II M2</v>
       </c>
     </row>
     <row r="83">
       <c r="A83">
-        <v>337255</v>
+        <v>336347</v>
       </c>
       <c r="B83" t="str">
         <v>H</v>
       </c>
       <c r="C83" t="str">
-        <v>M18</v>
+        <v>4L</v>
       </c>
       <c r="D83" t="str">
-        <v>2023 | M18</v>
+        <v>2023 | 4L</v>
       </c>
       <c r="E83" t="str">
-        <v>dim.</v>
+        <v>mar.</v>
       </c>
       <c r="F83" s="1">
-        <v>45354.375</v>
+        <v>45328.854166666664</v>
       </c>
       <c r="G83" t="str">
         <v>VBC Lausanne</v>
       </c>
       <c r="H83" t="str">
-        <v>Lausanne M18G</v>
+        <v>Lausanne III M4</v>
       </c>
       <c r="I83" t="str">
-        <v>Lutry-Lavaux M18G</v>
+        <v>La Tour M4</v>
       </c>
       <c r="J83" t="str">
         <v>Salle omnisports de Grand-Vennes 1</v>
       </c>
       <c r="K83" t="str">
-        <v>VBC Lausanne</v>
+        <v>Lausanne II M2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>